<commit_message>
daily Invoice Scraping project work
</commit_message>
<xml_diff>
--- a/Invoice Scraping/data_folder/JaneDoe_130792.xlsx
+++ b/Invoice Scraping/data_folder/JaneDoe_130792.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FLI028\Desktop\RPA_projects\Invoice Scraping\data_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171CA956-B486-4018-988B-C7C53D3BF222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E15DC1-5CA8-4CEE-B912-49E0E0C71F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1330" yWindow="750" windowWidth="14400" windowHeight="7820" xr2:uid="{36CCA0BA-31DE-4DFC-9418-7BB54E9A1907}"/>
+    <workbookView xWindow="1330" yWindow="750" windowWidth="14400" windowHeight="7820" xr2:uid="{99255164-9509-4F45-B292-BA09EAE9D405}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,28 +42,28 @@
     <t>InvoiceDate</t>
   </si>
   <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Sep 01, 2020</t>
   </si>
   <si>
-    <t>ItemNo</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>SubTotal</t>
-  </si>
-  <si>
-    <t>GST</t>
-  </si>
-  <si>
-    <t>Total</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
   <si>
     <t xml:space="preserve">4Tech keyboard black </t>
@@ -444,8 +444,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4DDDA0-5B7A-4A1A-9A1A-7FB4CA1FEF5D}">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053A5766-F39D-436E-8454-B0A23C88D514}">
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -459,25 +459,42 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>600</v>
+      </c>
+      <c r="G2">
+        <v>600</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -485,149 +502,130 @@
         <v>130792</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>900</v>
+      </c>
+      <c r="G3">
+        <v>900</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
+      <c r="F4">
+        <v>7800</v>
+      </c>
+      <c r="G4">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="F5">
+        <v>1500</v>
+      </c>
+      <c r="G5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
         <v>600</v>
       </c>
-      <c r="E4">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="G6">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
+      <c r="F7">
+        <v>1500</v>
+      </c>
+      <c r="G7">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
         <v>1</v>
       </c>
-      <c r="D5">
-        <v>900</v>
-      </c>
-      <c r="E5">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>7800</v>
-      </c>
-      <c r="E6">
-        <v>7800</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1500</v>
-      </c>
-      <c r="E7">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>600</v>
-      </c>
-      <c r="E8">
-        <v>1200</v>
+      <c r="F8">
+        <v>2000</v>
+      </c>
+      <c r="G8">
+        <v>2000</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>1500</v>
-      </c>
-      <c r="E9">
-        <v>3000</v>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9">
+        <v>17000</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>2000</v>
-      </c>
-      <c r="E10">
-        <v>2000</v>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10">
+        <v>1360</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12">
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D13" t="s">
+      <c r="F11" t="s">
         <v>19</v>
       </c>
-      <c r="E13">
+      <c r="G11">
         <v>18360</v>
       </c>
     </row>

</xml_diff>